<commit_message>
Update the Evidence Format for Stage 1
</commit_message>
<xml_diff>
--- a/nodestake/evidence.xlsx
+++ b/nodestake/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wubinbin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wubinbin/Downloads/GoN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEC58A8-5120-FE46-A8AB-E4D2E53F8427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A395D74-75F3-CB49-9765-62A85C59DE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="500" windowWidth="20480" windowHeight="16400" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="21420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
   <si>
     <t>TeamName</t>
   </si>
@@ -83,12 +83,6 @@
   </si>
   <si>
     <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
   </si>
   <si>
     <t>ibc class on chain</t>
@@ -618,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -662,28 +656,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
         <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +708,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -748,7 +742,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -782,7 +776,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -816,7 +810,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -850,20 +844,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -894,20 +888,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -938,20 +932,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -982,20 +976,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1026,20 +1020,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1070,20 +1064,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1092,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1116,10 +1110,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1150,20 +1144,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1194,20 +1188,20 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1232,12 +1226,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1268,12 +1262,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1304,12 +1298,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1340,12 +1334,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1386,35 +1380,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1454,16 +1448,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1503,16 +1497,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1524,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1550,32 +1544,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1587,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1615,32 +1595,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>41</v>
+      <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1637,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1705,7 +1671,7 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Stage 1 and Stage 2
fixed Stage 1 evidence format,
Add Stage 2
</commit_message>
<xml_diff>
--- a/nodestake/evidence.xlsx
+++ b/nodestake/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wubinbin/Downloads/GoN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A395D74-75F3-CB49-9765-62A85C59DE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7238941-DCF0-1543-934C-AAEA88A21F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="21420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="500" windowWidth="14400" windowHeight="21440" tabRatio="500" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,12 @@
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
   <si>
     <t>TeamName</t>
   </si>
@@ -82,21 +82,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -193,6 +178,214 @@
   </si>
   <si>
     <t>gon-irishub-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nodestakeNFTA7</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-120/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/nodestakeNFT</t>
+  </si>
+  <si>
+    <t>nodestakeNFTA8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-transfer/channel-0/nft-transfer/channel-41/nft-transfer/channel-3/nodestakeNFT</t>
+  </si>
+  <si>
+    <t>nodestakeNFTA9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-transfer/channel-17/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-120/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/nodestakeNFT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nodestakeNFTA10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-44/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/nodestakeNFT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nodestakeNFTA11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-transfer/channel-22/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-41/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/nodestakeNFT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nodestakeNFTA12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-41/nft-transfer/channel-6/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/nodestakeNFT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>3CEC4F61892C6DCCCAD0ABC042645587ECC33D8B2AA63FC06E67E14469DDFE05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>39D3392A0384E36C1FE80818675305EC645FE35E7F3DE2FB6A6E5CED588ED1A9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>14EDB7F484A3B12876D181A4A41A121B520E4FAA5E9718F90D1B8C3959D8D801</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCE44908E9BE598A881702B4355C7118FA16C279BBAF66828BE4EFB0875B9203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>\</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>6C922DE057440128C6FC93AD89659A4214CA31B0698F82445255AAEBB630302E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>906C1E71DEEA9AF9710FDE0B9DE2EBC48EFF75BF4889D4E18B382FE35EEC5354</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4A8D93BF303684F1E72F8EB388144771BE2E723D3D87AEF7946D5F977BD99911</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2179F3E5C4024A93D9CCE9B36F31C71D583CA196DEE880743EA9C51FCC454C7E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>496C36DA845F451F14365BF18A72FC514C6FF4DB44A9FE0F21277005585682CB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4C11252556B25AD201062D93C51468F6B1AABAA27291510FF8AE604A0C57C9CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50CB7320C4A931CE0A083AA83FA4E0BF4963F51C83E4AD1E89D337D32E5E5794</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>25F74DB13A4C36F5EF9C848ACED621E9A289255DC009A2573C4E56BFB67A6625</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D2862520365C3B3AB76CF41440AAB40E6118269B53F9698BF929FBE428DA673D</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DE6A216A8F560EA3151AEAFE628FB3122EDF919A7BBC0BDE24D5F3430460D52A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D8CB20625BE7D4CD2DAB3A7A25FA82D78DE87B512443665A14D6101F9B499A23</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>31966A742CEB6F97941535CD70E1AAD8FFD96D547D054DF02C9B40D719AAE1A7</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFE1CF178A826B3CBE77B1727B6877CA8C3EEE75818AD2B8DF40006DBDD14904</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>931303554587DD41EE68E6182268EAD9F17825F3A93F1766BFCCE51CA44555B1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>351AAFF6F13E4801DFD4EDC47A017274E12B79C96E5CCE818ACA6C871E619B22</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F7E908AF17D3D0ED665793219903DB91692659676A0D6161264EE17B4A9394B2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFB6148A96D473964254DB11EFF35C94CCE18538C9CD4EF8FB60E74715CB9971</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA4F5FE4441715CCC0BD22DFAB50DA66EA2BD9A7B4614B0745F4E34BBE488651</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2A414E17D1A26AB7F38FEE52A4DD0C75693C24A98D8CD624C7FF0747A49E0E46</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E9B60AC902174A5E188BF97D7D6944E309EC00BD665A5F68FD50C687AC1728D3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EA5A5A3672D9E6D73068C788FD08E737B497A549DCAC382452B32AC7906ADC59</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C09D594C8216C4482F1F9512F8B46E778C5EF3970AFF849956BD28938C44E8AB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E0744F834D2027B63A4F2B26311ECDF4C9B905D1E67739FB12A80184BCE59C3B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8FF4DBEA5FBA7F8074396D489645D66689AAD8DB59333FC3B8A8042B8DD048FA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>76ED6468F7D4258D3AEF048E6F296382E8FC1F001A333C1A362ADE67648C027C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1E4FA9EC2213998D3EFBC37CAC802F44DFD92D0E6EB3555FBBC920E6310201D9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4DF127AA7973EA8DC113C96872B98CFF600CFDDCDFD2DCB3796624052DAB5234</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>21AFB02009CC58C9F80394974C0BE5CF0659013A7E02E016B475B1536D309CDC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0364B6286F5B98E09056049DA26072D12D6824B739EE0E10AAAA2A70D54FAE73</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0FF4E2AA6E4D94405F1A5D174B502D9036B13492FF3D64680DE5EB46ABE6C13A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D51C3553EFBF2213AE746F7488BAA66C0DE4FC5EBD35E5B7B071E4817DC64F1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A3AB1D4228239D382721BBB133FBC3AF1564724F6412C0AAC7BC86029B9ABECB</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -200,7 +393,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -231,8 +424,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +448,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +478,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -612,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -656,28 +872,28 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +907,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -708,10 +926,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -725,7 +943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -742,10 +962,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -776,10 +998,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -793,7 +1015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -810,10 +1034,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -825,9 +1049,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -844,20 +1070,34 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -869,9 +1109,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -888,20 +1130,39 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>62</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -913,9 +1174,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -932,20 +1195,34 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>66</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -957,9 +1234,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -976,20 +1255,34 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1001,9 +1294,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1020,20 +1315,34 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>76</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>74</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1045,9 +1354,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1064,20 +1375,34 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>77</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>79</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1110,10 +1435,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1125,9 +1450,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1144,20 +1471,50 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>86</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14">
+      <c r="A5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14">
+      <c r="A6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14">
+      <c r="A7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1169,9 +1526,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1188,20 +1547,50 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1226,12 +1615,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1262,12 +1651,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1298,12 +1687,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1334,12 +1723,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1380,35 +1769,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1448,16 +1837,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1497,16 +1886,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1546,16 +1935,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1597,16 +1986,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +2009,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1637,10 +2028,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +2045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1671,10 +2064,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>